<commit_message>
update: latest kimai data pull for pay period 21
</commit_message>
<xml_diff>
--- a/kimai-data/21/pay-period-21.xlsx
+++ b/kimai-data/21/pay-period-21.xlsx
@@ -477,16 +477,16 @@
         <f>F6 + G6</f>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H6">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I6" t="str">
-        <v/>
+        <v>Extra 8.00 hours carry over</v>
       </c>
     </row>
     <row r="7">
@@ -593,16 +593,16 @@
         <f>F10 + G10</f>
       </c>
       <c r="F10">
-        <v>50.25</v>
+        <v>54.25</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
       <c r="H10">
-        <v>40.25</v>
+        <v>44.25</v>
       </c>
       <c r="I10" t="str">
-        <v/>
+        <v>Extra 4.25 hours carry over</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
refactor: migrate from pnpm to npm and update cron schedules
- Remove all pnpm references from codebase
- Update package.json to remove packageManager field
- Regenerate package-lock.json with npm
- Update all documentation to use npm commands
- Update cron schedules:
  - Monday reminder: 12 AM CST (midnight)
  - Daily reminder: 11 AM CST
- Update install scripts and error messages
- Clean up .slugignore file
</commit_message>
<xml_diff>
--- a/kimai-data/21/pay-period-21.xlsx
+++ b/kimai-data/21/pay-period-21.xlsx
@@ -477,16 +477,16 @@
         <f>F6 + G6</f>
       </c>
       <c r="F6">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G6">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H6">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I6" t="str">
-        <v>Extra 8.00 hours carry over</v>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -535,16 +535,16 @@
         <f>F8 + G8</f>
       </c>
       <c r="F8">
-        <v>89.5</v>
+        <v>81.5</v>
       </c>
       <c r="G8">
-        <v>44.75</v>
+        <v>40.75</v>
       </c>
       <c r="H8">
-        <v>44.75</v>
+        <v>40.75</v>
       </c>
       <c r="I8" t="str">
-        <v>Extra 9.50 hours carry over</v>
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -593,16 +593,16 @@
         <f>F10 + G10</f>
       </c>
       <c r="F10">
-        <v>54.25</v>
+        <v>50.25</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
       <c r="H10">
-        <v>44.25</v>
+        <v>40.25</v>
       </c>
       <c r="I10" t="str">
-        <v>Extra 4.25 hours carry over</v>
+        <v/>
       </c>
     </row>
     <row r="11">

</xml_diff>